<commit_message>
added examples for all profiles, edited medication guidance
</commit_message>
<xml_diff>
--- a/docs/CodeSystem-cibmtr-cadsr-cde.xlsx
+++ b/docs/CodeSystem-cibmtr-cadsr-cde.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-08-31T14:35:45-05:00</t>
+    <t>2022-09-02T15:43:08-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -129,61 +129,61 @@
     <t>1</t>
   </si>
   <si>
-    <t>$CADSR:2603692</t>
+    <t>2603692</t>
   </si>
   <si>
     <t>Acute Graft Versus Host Disease Maximum Overall Grade</t>
   </si>
   <si>
-    <t>$CADSR:2626409</t>
+    <t>2626409</t>
   </si>
   <si>
     <t>Biopsy Anatomic Site Performed Name</t>
   </si>
   <si>
-    <t>$CADSR:2797618</t>
+    <t>2797618</t>
   </si>
   <si>
     <t>Acute Graft Versus Host Disease Skin Involvement Maximum Severity Type</t>
   </si>
   <si>
-    <t>$CADSR:2797633</t>
+    <t>2797633</t>
   </si>
   <si>
     <t>Acute Graft Versus Host Disease Lower Gastrointestinal Tract Involvement Maximum Severity Type</t>
   </si>
   <si>
-    <t>$CADSR:2797671</t>
+    <t>2797671</t>
   </si>
   <si>
     <t>Acute Graft Versus Host Disease Liver Involvement Maximum Severity Type</t>
   </si>
   <si>
-    <t>$CADSR:2980753</t>
+    <t>2980753</t>
   </si>
   <si>
     <t>Therapeutic Procedure Administered Type</t>
   </si>
   <si>
-    <t>$CADSR:3005293</t>
+    <t>3005293</t>
   </si>
   <si>
     <t>Graft Versus Host Disease Diagnosis Type</t>
   </si>
   <si>
-    <t>$CADSR:5040179</t>
+    <t>5040179</t>
   </si>
   <si>
     <t>Acute Graft Versus Host Disease Stage Upper Gastrointestinal Tract Severity Type</t>
   </si>
   <si>
-    <t>$CADSR:5263856</t>
+    <t>5263856</t>
   </si>
   <si>
     <t>Post Infusion Procedure Timepoint Type</t>
   </si>
   <si>
-    <t>$CADSR:6975011</t>
+    <t>6975011</t>
   </si>
   <si>
     <t>Concomitant Medication Use Indication Reason</t>

</xml_diff>